<commit_message>
added dc removal on the FFT for velocity
</commit_message>
<xml_diff>
--- a/Velocity/Heterodyne/Charaterisations/ADC FFT Calibration.xlsx
+++ b/Velocity/Heterodyne/Charaterisations/ADC FFT Calibration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ad.monash.edu\home\User070\scat0009\Documents\Monash-BoSL\Velocity\Heterodyne\Charaterisations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F195393-64E7-4A7C-A433-FA8B824DE686}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E13CCBB-EC6E-4668-8B9F-290CFE8667B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14205" xr2:uid="{154B11D8-0F49-4F86-9276-DD7AC67C7F4A}"/>
   </bookViews>
@@ -2907,7 +2907,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y9" sqref="Y9"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>